<commit_message>
integrate 1872 law, data file, write csv all laws, and update instrumental_var data
</commit_message>
<xml_diff>
--- a/data/polid_data/instrumental_variable_est.xlsx
+++ b/data/polid_data/instrumental_variable_est.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2651" uniqueCount="1902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2731" uniqueCount="1956">
   <si>
     <t>polid</t>
   </si>
@@ -5758,6 +5758,168 @@
   <si>
     <t>van Stapele</t>
   </si>
+  <si>
+    <t>00154</t>
+  </si>
+  <si>
+    <t>Bomans</t>
+  </si>
+  <si>
+    <t>Journalist</t>
+  </si>
+  <si>
+    <t>00341</t>
+  </si>
+  <si>
+    <t>Dresselhuys</t>
+  </si>
+  <si>
+    <t>00968</t>
+  </si>
+  <si>
+    <t>01334</t>
+  </si>
+  <si>
+    <t>Van Sypesteyn</t>
+  </si>
+  <si>
+    <t>00009</t>
+  </si>
+  <si>
+    <t>Taets van Amerongen</t>
+  </si>
+  <si>
+    <t>01092</t>
+  </si>
+  <si>
+    <t>Van Reenen</t>
+  </si>
+  <si>
+    <t>01065</t>
+  </si>
+  <si>
+    <t>Pyls</t>
+  </si>
+  <si>
+    <t>01316</t>
+  </si>
+  <si>
+    <t>Storm van 's-Gravezande</t>
+  </si>
+  <si>
+    <t>00437</t>
+  </si>
+  <si>
+    <t>00538</t>
+  </si>
+  <si>
+    <t>Heemskerk Az.</t>
+  </si>
+  <si>
+    <t>00573</t>
+  </si>
+  <si>
+    <t>van den Heuvel</t>
+  </si>
+  <si>
+    <t>01281</t>
+  </si>
+  <si>
+    <t>Smitz</t>
+  </si>
+  <si>
+    <t>00674</t>
+  </si>
+  <si>
+    <t>Kappeyne van de Coppello</t>
+  </si>
+  <si>
+    <t>Rector</t>
+  </si>
+  <si>
+    <t>00857</t>
+  </si>
+  <si>
+    <t>Van Lynden van Sandenburg</t>
+  </si>
+  <si>
+    <t>00765</t>
+  </si>
+  <si>
+    <t>Van Kuyk</t>
+  </si>
+  <si>
+    <t>00322</t>
+  </si>
+  <si>
+    <t>van der Does de Willebois</t>
+  </si>
+  <si>
+    <t>00870</t>
+  </si>
+  <si>
+    <t>van der Maesen de Sombreff</t>
+  </si>
+  <si>
+    <t>01603</t>
+  </si>
+  <si>
+    <t>van Zuylen van Nyevelt</t>
+  </si>
+  <si>
+    <t>00350</t>
+  </si>
+  <si>
+    <t>Dumbar</t>
+  </si>
+  <si>
+    <t>00631</t>
+  </si>
+  <si>
+    <t>s Jacob</t>
+  </si>
+  <si>
+    <t>00130</t>
+  </si>
+  <si>
+    <t>Blom</t>
+  </si>
+  <si>
+    <t>01123</t>
+  </si>
+  <si>
+    <t>de Roo van Alderwerelt</t>
+  </si>
+  <si>
+    <t>00878</t>
+  </si>
+  <si>
+    <t>du Marchie van Voorthuysen</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>01272</t>
+  </si>
+  <si>
+    <t>00784</t>
+  </si>
+  <si>
+    <t>de Lange</t>
+  </si>
+  <si>
+    <t>00828</t>
+  </si>
+  <si>
+    <t>van der Linden</t>
+  </si>
+  <si>
+    <t>Heemskerk Bz.</t>
+  </si>
+  <si>
+    <t>Bankier</t>
+  </si>
 </sst>
 </file>
 
@@ -5768,7 +5930,7 @@
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
@@ -5824,7 +5986,6 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -5840,7 +6001,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5924,13 +6085,10 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -15542,7 +15700,7 @@
       <c r="F253" s="19" t="s">
         <v>1814</v>
       </c>
-      <c r="G253" s="29">
+      <c r="G253" s="12">
         <v>4.0</v>
       </c>
       <c r="H253" s="5"/>
@@ -15587,7 +15745,7 @@
       <c r="F254" s="18" t="s">
         <v>1822</v>
       </c>
-      <c r="G254" s="29">
+      <c r="G254" s="12">
         <v>2.0</v>
       </c>
       <c r="H254" s="5"/>
@@ -15638,10 +15796,10 @@
       <c r="F255" s="19" t="s">
         <v>1832</v>
       </c>
-      <c r="G255" s="29">
+      <c r="G255" s="12">
         <v>5.0</v>
       </c>
-      <c r="H255" s="30" t="s">
+      <c r="H255" s="5" t="s">
         <v>941</v>
       </c>
       <c r="I255" s="5" t="s">
@@ -15708,7 +15866,7 @@
       <c r="F257" s="19" t="s">
         <v>1844</v>
       </c>
-      <c r="G257" s="29">
+      <c r="G257" s="12">
         <v>0.0</v>
       </c>
       <c r="H257" s="5"/>
@@ -15785,7 +15943,7 @@
       <c r="F259" s="18">
         <v>3484.0</v>
       </c>
-      <c r="G259" s="29">
+      <c r="G259" s="12">
         <v>0.0</v>
       </c>
       <c r="H259" s="5"/>
@@ -15850,10 +16008,10 @@
       <c r="F261" s="19" t="s">
         <v>1870</v>
       </c>
-      <c r="G261" s="29">
+      <c r="G261" s="12">
         <v>10.0</v>
       </c>
-      <c r="H261" s="30" t="s">
+      <c r="H261" s="5" t="s">
         <v>1074</v>
       </c>
       <c r="I261" s="5" t="s">
@@ -15900,10 +16058,10 @@
       <c r="F262" s="19" t="s">
         <v>1878</v>
       </c>
-      <c r="G262" s="29">
+      <c r="G262" s="12">
         <v>12.0</v>
       </c>
-      <c r="H262" s="30" t="s">
+      <c r="H262" s="5" t="s">
         <v>1264</v>
       </c>
       <c r="I262" s="5" t="s">
@@ -15932,14 +16090,16 @@
       </c>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="A263" s="31" t="s">
+      <c r="A263" s="29" t="s">
         <v>1883</v>
       </c>
       <c r="B263" s="5" t="s">
         <v>1884</v>
       </c>
       <c r="F263" s="9"/>
-      <c r="G263" s="12"/>
+      <c r="G263" s="12">
+        <v>0.0</v>
+      </c>
       <c r="H263" s="5"/>
       <c r="I263" s="5" t="s">
         <v>1885</v>
@@ -15947,14 +16107,16 @@
       <c r="L263" s="1"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="A264" s="31" t="s">
+      <c r="A264" s="29" t="s">
         <v>1886</v>
       </c>
       <c r="B264" s="5" t="s">
         <v>1887</v>
       </c>
       <c r="F264" s="9"/>
-      <c r="G264" s="12"/>
+      <c r="G264" s="12">
+        <v>1.0</v>
+      </c>
       <c r="H264" s="5"/>
       <c r="I264" s="5" t="s">
         <v>104</v>
@@ -15962,14 +16124,16 @@
       <c r="L264" s="1"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="A265" s="31" t="s">
+      <c r="A265" s="29" t="s">
         <v>1888</v>
       </c>
       <c r="B265" s="5" t="s">
         <v>1889</v>
       </c>
       <c r="F265" s="9"/>
-      <c r="G265" s="12"/>
+      <c r="G265" s="12">
+        <v>5.0</v>
+      </c>
       <c r="H265" s="5"/>
       <c r="I265" s="5" t="s">
         <v>1890</v>
@@ -15977,14 +16141,16 @@
       <c r="L265" s="1"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="A266" s="31" t="s">
+      <c r="A266" s="29" t="s">
         <v>1241</v>
       </c>
       <c r="B266" s="5" t="s">
         <v>1891</v>
       </c>
       <c r="F266" s="9"/>
-      <c r="G266" s="12"/>
+      <c r="G266" s="12">
+        <v>0.0</v>
+      </c>
       <c r="H266" s="5"/>
       <c r="I266" s="5" t="s">
         <v>881</v>
@@ -15992,14 +16158,16 @@
       <c r="L266" s="1"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="A267" s="31" t="s">
+      <c r="A267" s="29" t="s">
         <v>1892</v>
       </c>
       <c r="B267" s="5" t="s">
         <v>1893</v>
       </c>
       <c r="F267" s="9"/>
-      <c r="G267" s="12"/>
+      <c r="G267" s="12">
+        <v>1.0</v>
+      </c>
       <c r="H267" s="5"/>
       <c r="I267" s="5" t="s">
         <v>881</v>
@@ -16007,14 +16175,16 @@
       <c r="L267" s="1"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="A268" s="31" t="s">
+      <c r="A268" s="29" t="s">
         <v>1894</v>
       </c>
       <c r="B268" s="5" t="s">
         <v>1895</v>
       </c>
       <c r="F268" s="9"/>
-      <c r="G268" s="12"/>
+      <c r="G268" s="12">
+        <v>1.0</v>
+      </c>
       <c r="H268" s="5"/>
       <c r="I268" s="5" t="s">
         <v>208</v>
@@ -16022,14 +16192,16 @@
       <c r="L268" s="1"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="A269" s="31" t="s">
+      <c r="A269" s="29" t="s">
         <v>1896</v>
       </c>
       <c r="B269" s="5" t="s">
         <v>1897</v>
       </c>
       <c r="F269" s="9"/>
-      <c r="G269" s="12"/>
+      <c r="G269" s="12">
+        <v>8.0</v>
+      </c>
       <c r="H269" s="5"/>
       <c r="I269" s="5" t="s">
         <v>881</v>
@@ -16037,14 +16209,16 @@
       <c r="L269" s="1"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="A270" s="31" t="s">
+      <c r="A270" s="29" t="s">
         <v>1898</v>
       </c>
       <c r="B270" s="5" t="s">
         <v>1899</v>
       </c>
       <c r="F270" s="9"/>
-      <c r="G270" s="12"/>
+      <c r="G270" s="12">
+        <v>0.0</v>
+      </c>
       <c r="H270" s="5"/>
       <c r="I270" s="5" t="s">
         <v>881</v>
@@ -16052,14 +16226,16 @@
       <c r="L270" s="1"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="A271" s="31" t="s">
+      <c r="A271" s="29" t="s">
         <v>1900</v>
       </c>
       <c r="B271" s="5" t="s">
         <v>1901</v>
       </c>
       <c r="F271" s="9"/>
-      <c r="G271" s="12"/>
+      <c r="G271" s="12">
+        <v>0.0</v>
+      </c>
       <c r="H271" s="5"/>
       <c r="I271" s="5" t="s">
         <v>881</v>
@@ -16067,138 +16243,382 @@
       <c r="L271" s="1"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
+      <c r="A272" s="29" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B272" s="5" t="s">
+        <v>1903</v>
+      </c>
       <c r="F272" s="9"/>
-      <c r="G272" s="12"/>
+      <c r="G272" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="I272" s="5" t="s">
+        <v>1904</v>
+      </c>
       <c r="L272" s="1"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
+      <c r="A273" s="29" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B273" s="5" t="s">
+        <v>1906</v>
+      </c>
       <c r="F273" s="9"/>
-      <c r="G273" s="10"/>
+      <c r="G273" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I273" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="L273" s="1"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
+      <c r="A274" s="29" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B274" s="5" t="s">
+        <v>1197</v>
+      </c>
       <c r="F274" s="9"/>
       <c r="G274" s="10"/>
+      <c r="I274" s="5" t="s">
+        <v>141</v>
+      </c>
       <c r="L274" s="1"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
+      <c r="A275" s="29" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B275" s="5" t="s">
+        <v>1909</v>
+      </c>
       <c r="F275" s="9"/>
       <c r="G275" s="10"/>
+      <c r="I275" s="5" t="s">
+        <v>208</v>
+      </c>
       <c r="L275" s="1"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
+      <c r="A276" s="29" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B276" s="5" t="s">
+        <v>1911</v>
+      </c>
       <c r="F276" s="9"/>
       <c r="G276" s="10"/>
+      <c r="I276" s="5" t="s">
+        <v>402</v>
+      </c>
       <c r="L276" s="1"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
+      <c r="A277" s="29" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B277" s="5" t="s">
+        <v>1913</v>
+      </c>
       <c r="F277" s="9"/>
       <c r="G277" s="10"/>
+      <c r="I277" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="L277" s="1"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
+      <c r="A278" s="29" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B278" s="5" t="s">
+        <v>1915</v>
+      </c>
       <c r="F278" s="9"/>
       <c r="G278" s="10"/>
+      <c r="I278" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="L278" s="1"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
+      <c r="A279" s="29" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B279" s="5" t="s">
+        <v>1917</v>
+      </c>
       <c r="F279" s="9"/>
       <c r="G279" s="10"/>
+      <c r="I279" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="L279" s="1"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
+      <c r="A280" s="29" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B280" s="5" t="s">
+        <v>220</v>
+      </c>
       <c r="F280" s="9"/>
       <c r="G280" s="10"/>
+      <c r="I280" s="5" t="s">
+        <v>402</v>
+      </c>
       <c r="L280" s="1"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
+      <c r="A281" s="29" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B281" s="5" t="s">
+        <v>1920</v>
+      </c>
       <c r="F281" s="9"/>
       <c r="G281" s="10"/>
       <c r="L281" s="1"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
+      <c r="A282" s="29" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>1922</v>
+      </c>
       <c r="F282" s="9"/>
       <c r="G282" s="10"/>
+      <c r="I282" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="L282" s="1"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
+      <c r="A283" s="29" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>1924</v>
+      </c>
       <c r="F283" s="9"/>
       <c r="G283" s="10"/>
+      <c r="I283" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="L283" s="1"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
+      <c r="A284" s="29" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>1926</v>
+      </c>
       <c r="F284" s="9"/>
       <c r="G284" s="10"/>
+      <c r="I284" s="5" t="s">
+        <v>1927</v>
+      </c>
       <c r="L284" s="1"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
+      <c r="A285" s="29" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B285" s="5" t="s">
+        <v>1929</v>
+      </c>
       <c r="F285" s="9"/>
       <c r="G285" s="10"/>
+      <c r="I285" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="L285" s="1"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
+      <c r="A286" s="29" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>1931</v>
+      </c>
       <c r="F286" s="9"/>
       <c r="G286" s="10"/>
+      <c r="I286" s="5" t="s">
+        <v>1010</v>
+      </c>
       <c r="L286" s="1"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
+      <c r="A287" s="29" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>1933</v>
+      </c>
       <c r="F287" s="9"/>
       <c r="G287" s="10"/>
+      <c r="I287" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="L287" s="1"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
+      <c r="A288" s="29" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B288" s="5" t="s">
+        <v>1935</v>
+      </c>
       <c r="F288" s="9"/>
       <c r="G288" s="10"/>
+      <c r="I288" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="L288" s="1"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
+      <c r="A289" s="29" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B289" s="5" t="s">
+        <v>1937</v>
+      </c>
       <c r="F289" s="9"/>
       <c r="G289" s="10"/>
+      <c r="I289" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="L289" s="1"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
+      <c r="A290" s="29" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>1939</v>
+      </c>
       <c r="F290" s="9"/>
       <c r="G290" s="10"/>
+      <c r="I290" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="L290" s="1"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
+      <c r="A291" s="29" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B291" s="30" t="s">
+        <v>1941</v>
+      </c>
       <c r="F291" s="9"/>
       <c r="G291" s="10"/>
+      <c r="I291" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="L291" s="1"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
+      <c r="A292" s="29" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B292" s="5" t="s">
+        <v>1943</v>
+      </c>
       <c r="F292" s="9"/>
       <c r="G292" s="10"/>
+      <c r="I292" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="L292" s="1"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
+      <c r="A293" s="29" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B293" s="5" t="s">
+        <v>1945</v>
+      </c>
       <c r="F293" s="9"/>
       <c r="G293" s="10"/>
+      <c r="I293" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="L293" s="1"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
+      <c r="A294" s="29" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B294" s="5" t="s">
+        <v>1947</v>
+      </c>
       <c r="F294" s="9"/>
       <c r="G294" s="10"/>
+      <c r="I294" s="5" t="s">
+        <v>1948</v>
+      </c>
       <c r="L294" s="1"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
+      <c r="A295" s="29" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B295" s="5" t="s">
+        <v>1517</v>
+      </c>
       <c r="F295" s="9"/>
       <c r="G295" s="10"/>
+      <c r="I295" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="L295" s="1"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
+      <c r="A296" s="29" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B296" s="5" t="s">
+        <v>1951</v>
+      </c>
       <c r="F296" s="9"/>
       <c r="G296" s="10"/>
+      <c r="I296" s="5" t="s">
+        <v>318</v>
+      </c>
       <c r="L296" s="1"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
+      <c r="A297" s="29" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B297" s="5" t="s">
+        <v>1953</v>
+      </c>
       <c r="F297" s="9"/>
       <c r="G297" s="10"/>
+      <c r="I297" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="L297" s="1"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
+      <c r="A298" s="29" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B298" s="5" t="s">
+        <v>1954</v>
+      </c>
       <c r="F298" s="9"/>
       <c r="G298" s="10"/>
+      <c r="I298" s="5" t="s">
+        <v>1955</v>
+      </c>
       <c r="L298" s="1"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
@@ -19695,11 +20115,6 @@
       <c r="F997" s="9"/>
       <c r="G997" s="10"/>
       <c r="L997" s="1"/>
-    </row>
-    <row r="998" ht="15.75" customHeight="1">
-      <c r="F998" s="9"/>
-      <c r="G998" s="10"/>
-      <c r="L998" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>